<commit_message>
Migrate from SQL Server to MySQL.
</commit_message>
<xml_diff>
--- a/BTS.Web/AppFiles/Tmp/User List Sample.xlsx
+++ b/BTS.Web/AppFiles/Tmp/User List Sample.xlsx
@@ -1418,7 +1418,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1035" name="Picture 2"/>
+        <xdr:cNvPr id="1036" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1770,7 +1770,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>